<commit_message>
Merging emission rates, lab based chemistry, and field observations.
</commit_message>
<xml_diff>
--- a/inputData/nla2017/nla17lakeNumberAndArea.xlsx
+++ b/inputData/nla2017/nla17lakeNumberAndArea.xlsx
@@ -1257,8 +1257,8 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="13" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eecf5014d928db928e813ac0cc0f25c5">
-  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="ae092a53b8b494863c1d9d9bfd6cbaf0" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
+<ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101001AF5FC5DD832BE4DBA6B24560DD3ADC0" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="812b8335a1076cc0735232c21164ce2d">
+  <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4" xmlns:ns3="http://schemas.microsoft.com/sharepoint.v3" xmlns:ns4="http://schemas.microsoft.com/sharepoint/v3/fields" xmlns:ns5="8b03727f-4454-4722-b3e6-018d8dcaf2fd" xmlns:ns6="ed970698-2d60-4bab-a048-d9be527522d9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="241c6c65034c5d3b3239e7a72dd7aed1" ns1:_="" ns2:_="" ns3:_="" ns4:_="" ns5:_="" ns6:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
     <xsd:import namespace="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint.v3"/>
@@ -1299,6 +1299,9 @@
                 <xsd:element ref="ns6:MediaServiceOCR" minOccurs="0"/>
                 <xsd:element ref="ns6:MediaServiceAutoKeyPoints" minOccurs="0"/>
                 <xsd:element ref="ns6:MediaServiceKeyPoints" minOccurs="0"/>
+                <xsd:element ref="ns6:MediaServiceLocation" minOccurs="0"/>
+                <xsd:element ref="ns6:MediaLengthInSeconds" minOccurs="0"/>
+                <xsd:element ref="ns6:lcf76f155ced4ddcb4097134ff3c332f" minOccurs="0"/>
               </xsd:all>
             </xsd:complexType>
           </xsd:element>
@@ -1594,6 +1597,23 @@
           <xsd:maxLength value="255"/>
         </xsd:restriction>
       </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaServiceLocation" ma:index="39" nillable="true" ma:displayName="Location" ma:internalName="MediaServiceLocation" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Text"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="MediaLengthInSeconds" ma:index="40" nillable="true" ma:displayName="Length (seconds)" ma:internalName="MediaLengthInSeconds" ma:readOnly="true">
+      <xsd:simpleType>
+        <xsd:restriction base="dms:Unknown"/>
+      </xsd:simpleType>
+    </xsd:element>
+    <xsd:element name="lcf76f155ced4ddcb4097134ff3c332f" ma:index="42" nillable="true" ma:taxonomy="true" ma:internalName="lcf76f155ced4ddcb4097134ff3c332f" ma:taxonomyFieldName="MediaServiceImageTags" ma:displayName="Image Tags" ma:readOnly="false" ma:fieldId="{5cf76f15-5ced-4ddc-b409-7134ff3c332f}" ma:taxonomyMulti="true" ma:sspId="29f62856-1543-49d4-a736-4569d363f533" ma:termSetId="09814cd3-568e-fe90-9814-8d621ff8fb84" ma:anchorId="fba54fb3-c3e1-fe81-a776-ca4b69148c4d" ma:open="true" ma:isKeyword="false">
+      <xsd:complexType>
+        <xsd:sequence>
+          <xsd:element ref="pc:Terms" minOccurs="0" maxOccurs="1"/>
+        </xsd:sequence>
+      </xsd:complexType>
     </xsd:element>
   </xsd:schema>
   <xsd:schema xmlns="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:dc="http://purl.org/dc/elements/1.1/" xmlns:dcterms="http://purl.org/dc/terms/" xmlns:odoc="http://schemas.microsoft.com/internal/obd" targetNamespace="http://schemas.openxmlformats.org/package/2006/metadata/core-properties" elementFormDefault="qualified" attributeFormDefault="unqualified" blockDefault="#all">
@@ -1744,12 +1764,15 @@
       </UserInfo>
     </EPA_x0020_Contributor>
     <TaxCatchAll xmlns="4ffa91fb-a0ff-4ac5-b2db-65c790d184a4"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="ed970698-2d60-4bab-a048-d9be527522d9">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{FB5B9414-B4EA-4371-8E3D-6AD07CFC4F96}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A271B58A-D291-435A-AE5C-44CA8D6C6997}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>

</xml_diff>